<commit_message>
fix report for group100 for freezed
</commit_message>
<xml_diff>
--- a/storage/app/reports/التقرير الأسبوعي-17.xlsx
+++ b/storage/app/reports/التقرير الأسبوعي-17.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>متوسط النقاط</t>
   </si>
@@ -33,7 +33,7 @@
     <t>صفحات الحفظ</t>
   </si>
   <si>
-    <t>14.29 %</t>
+    <t>18.18 %</t>
   </si>
   <si>
     <t>نسبة الطلاب المجمدين</t>
@@ -42,7 +42,7 @@
     <t>عدد الطلاب المجمدين</t>
   </si>
   <si>
-    <t>78.57 %</t>
+    <t>63.64 %</t>
   </si>
   <si>
     <t>نسبة التسميع</t>
@@ -66,55 +66,40 @@
     <t>ليس لديه مشرف</t>
   </si>
   <si>
-    <t>عبد القادر عبد الهادي السعيد</t>
-  </si>
-  <si>
-    <t>عقل جابر الفيفي</t>
-  </si>
-  <si>
-    <t>موقوف</t>
+    <t>رامز شافع الخالدي</t>
+  </si>
+  <si>
+    <t>مجمد</t>
+  </si>
+  <si>
+    <t>مسؤول الطلاب للذكور</t>
+  </si>
+  <si>
+    <t>مسؤول لجنة إعلامية</t>
   </si>
   <si>
     <t>مشرف</t>
   </si>
   <si>
-    <t>عبد الكريم حسام مدني</t>
-  </si>
-  <si>
-    <t>منسحب</t>
-  </si>
-  <si>
-    <t>باهر غيد السعيد</t>
-  </si>
-  <si>
     <t>رئيس ملتقى القرآن الكريم</t>
   </si>
   <si>
+    <t>ابان راضي باشا</t>
+  </si>
+  <si>
+    <t>نائب رئيس ملتقى القرآن الكريم</t>
+  </si>
+  <si>
+    <t>نظام كرم السويلم</t>
+  </si>
+  <si>
+    <t>آدم وفاء العنزي</t>
+  </si>
+  <si>
     <t>عضو لجنة متابعة</t>
   </si>
   <si>
-    <t>حسن مريم الحنتوشي</t>
-  </si>
-  <si>
-    <t>عبد العفو غيداء القحطاني</t>
-  </si>
-  <si>
-    <t>راغب ميس السماعيل</t>
-  </si>
-  <si>
-    <t>رامي داليا السالم</t>
-  </si>
-  <si>
-    <t>أمجد العزم العسكر</t>
-  </si>
-  <si>
-    <t>مجمد</t>
-  </si>
-  <si>
-    <t>عزالدين ايمن الخالدي</t>
-  </si>
-  <si>
-    <t>نائب رئيس ملتقى القرآن الكريم</t>
+    <t>مصعب عبد الكريم العقل</t>
   </si>
   <si>
     <t>النقاط</t>
@@ -153,7 +138,7 @@
     <t>أولا: تقرير التسميع الأسبوعي</t>
   </si>
   <si>
-    <t>التسميع الأسبوعي لملتقى القرآن الكريم (ذكور) في الفترة من 2024-04-06 إلى 2024-04-12</t>
+    <t>التسميع الأسبوعي لملتقى القرآن الكريم (ذكور) في الفترة من 2024-05-04 إلى 2024-05-10</t>
   </si>
   <si>
     <t>نسبة التسميع 100%</t>
@@ -655,17 +640,17 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" rightToLeft="true">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" spans="1:12">
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -694,7 +679,7 @@
     <row r="4" spans="1:12"/>
     <row r="5" spans="1:12">
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -723,37 +708,37 @@
     <row r="7" spans="1:12"/>
     <row r="8" spans="1:12">
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -761,10 +746,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4">
-        <v>22012233</v>
+        <v>26753970</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>15</v>
@@ -773,22 +758,22 @@
         <v>14</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="H9" s="4">
         <v>5</v>
       </c>
       <c r="I9" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J9" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K9" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L9" s="4">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -796,10 +781,10 @@
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D10" s="4">
-        <v>69921491</v>
+        <v>22014233</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>15</v>
@@ -808,13 +793,13 @@
         <v>14</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="H10" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I10" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J10" s="4">
         <v>9</v>
@@ -823,7 +808,7 @@
         <v>7</v>
       </c>
       <c r="L10" s="4">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -831,10 +816,10 @@
         <v>3</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D11" s="4">
-        <v>50863848</v>
+        <v>24264634</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>15</v>
@@ -849,16 +834,16 @@
         <v>4</v>
       </c>
       <c r="I11" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J11" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K11" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L11" s="4">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -866,10 +851,10 @@
         <v>4</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D12" s="4">
-        <v>58324885</v>
+        <v>33480892</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>15</v>
@@ -878,22 +863,22 @@
         <v>14</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
+        <v>3</v>
+      </c>
+      <c r="J12" s="4">
+        <v>10</v>
+      </c>
+      <c r="K12" s="4">
         <v>5</v>
       </c>
-      <c r="I12" s="4">
-        <v>5</v>
-      </c>
-      <c r="J12" s="4">
-        <v>8</v>
-      </c>
-      <c r="K12" s="4">
-        <v>1</v>
-      </c>
       <c r="L12" s="4">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -901,10 +886,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D13" s="4">
-        <v>21272252</v>
+        <v>22012233</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>15</v>
@@ -916,19 +901,19 @@
         <v>13</v>
       </c>
       <c r="H13" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I13" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J13" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K13" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L13" s="4">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -936,10 +921,10 @@
         <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D14" s="4">
-        <v>86088377</v>
+        <v>76107628</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>15</v>
@@ -948,22 +933,22 @@
         <v>14</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H14" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I14" s="4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J14" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K14" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L14" s="4">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -971,10 +956,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D15" s="4">
-        <v>62492923</v>
+        <v>22011233</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>15</v>
@@ -986,389 +971,284 @@
         <v>13</v>
       </c>
       <c r="H15" s="4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I15" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J15" s="4">
+        <v>7</v>
+      </c>
+      <c r="K15" s="4">
+        <v>2</v>
+      </c>
+      <c r="L15" s="4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="B16" s="5">
+        <v>8</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="5">
+        <v>22013233</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="B17" s="5">
         <v>9</v>
       </c>
-      <c r="K15" s="4">
-        <v>4</v>
-      </c>
-      <c r="L15" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="B16" s="4">
-        <v>8</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="4">
-        <v>22014233</v>
-      </c>
-      <c r="E16" s="4" t="s">
+      <c r="C17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="5">
+        <v>22016233</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="4">
-        <v>4</v>
-      </c>
-      <c r="I16" s="4">
-        <v>1</v>
-      </c>
-      <c r="J16" s="4">
-        <v>4</v>
-      </c>
-      <c r="K16" s="4">
-        <v>8</v>
-      </c>
-      <c r="L16" s="4">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="B17" s="4">
-        <v>9</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="4">
-        <v>22011233</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="G17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="B18" s="5">
+        <v>10</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="5">
+        <v>22017233</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0</v>
+      </c>
+      <c r="L18" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="B19" s="5">
+        <v>11</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="5">
+        <v>28527252</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="4">
-        <v>2</v>
-      </c>
-      <c r="I17" s="4">
-        <v>2</v>
-      </c>
-      <c r="J17" s="4">
-        <v>1</v>
-      </c>
-      <c r="K17" s="4">
-        <v>10</v>
-      </c>
-      <c r="L17" s="4">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="B18" s="4">
-        <v>10</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="4">
-        <v>94335670</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="4">
-        <v>3</v>
-      </c>
-      <c r="I18" s="4">
-        <v>1</v>
-      </c>
-      <c r="J18" s="4">
-        <v>5</v>
-      </c>
-      <c r="K18" s="4">
-        <v>1</v>
-      </c>
-      <c r="L18" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="B19" s="4">
-        <v>11</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="4">
-        <v>87136127</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="4">
-        <v>2</v>
-      </c>
-      <c r="I19" s="4">
-        <v>2</v>
-      </c>
-      <c r="J19" s="4">
-        <v>3</v>
-      </c>
-      <c r="K19" s="4">
-        <v>4</v>
-      </c>
-      <c r="L19" s="4">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="B20" s="5">
+      <c r="H19" s="5">
+        <v>0</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0</v>
+      </c>
+      <c r="K19" s="5">
+        <v>0</v>
+      </c>
+      <c r="L19" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12"/>
+    <row r="21" spans="1:12">
+      <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="5">
-        <v>22013233</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="5">
-        <v>0</v>
-      </c>
-      <c r="I20" s="5">
-        <v>0</v>
-      </c>
-      <c r="J20" s="5">
-        <v>0</v>
-      </c>
-      <c r="K20" s="5">
-        <v>0</v>
-      </c>
-      <c r="L20" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="B21" s="5">
-        <v>13</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="5">
-        <v>92193185</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="5">
-        <v>0</v>
-      </c>
-      <c r="I21" s="5">
-        <v>0</v>
-      </c>
-      <c r="J21" s="5">
-        <v>0</v>
-      </c>
-      <c r="K21" s="5">
-        <v>0</v>
-      </c>
-      <c r="L21" s="5">
-        <v>0</v>
-      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="B22" s="5">
-        <v>14</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="5">
-        <v>48584616</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="5">
-        <v>0</v>
-      </c>
-      <c r="I22" s="5">
-        <v>0</v>
-      </c>
-      <c r="J22" s="5">
-        <v>0</v>
-      </c>
-      <c r="K22" s="5">
-        <v>0</v>
-      </c>
-      <c r="L22" s="5">
-        <v>0</v>
-      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
     </row>
     <row r="23" spans="1:12"/>
     <row r="24" spans="1:12">
-      <c r="B24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
+      <c r="B24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="3">
+        <v>11</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="3">
+        <v>7</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-    </row>
-    <row r="26" spans="1:12"/>
+      <c r="B25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="3">
+        <v>2</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="6"/>
+      <c r="J25" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="B26" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="3">
+        <v>19</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="3">
+        <v>1.73</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="3">
+        <v>1.73</v>
+      </c>
+    </row>
     <row r="27" spans="1:12">
       <c r="B27" s="6" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="3">
-        <v>14</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="3">
-        <v>11</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I27" s="6"/>
-      <c r="J27" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="B28" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="3">
-        <v>2</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="6"/>
-      <c r="G28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I28" s="6"/>
-      <c r="J28" s="3">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="B29" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="3">
-        <v>28</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F29" s="6"/>
-      <c r="G29" s="3">
-        <v>3.21</v>
-      </c>
-      <c r="H29" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" s="6"/>
-      <c r="J29" s="3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="B30" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="3">
-        <v>25.93</v>
+        <v>18.45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="B2:L3"/>
     <mergeCell ref="B5:L6"/>
-    <mergeCell ref="B24:L25"/>
+    <mergeCell ref="B21:L22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="H26:I26"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="B30:C30"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1391,7 +1271,7 @@
   <sheetData>
     <row r="2" spans="1:10">
       <c r="B2" s="7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -1416,10 +1296,10 @@
     <row r="4" spans="1:10"/>
     <row r="5" spans="1:10">
       <c r="B5" s="8" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8" t="s">
@@ -1427,7 +1307,7 @@
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="8" t="s">
@@ -1440,7 +1320,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9">
@@ -1461,7 +1341,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9">
@@ -1482,7 +1362,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="9">
@@ -1503,7 +1383,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9">
@@ -1524,7 +1404,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9">
@@ -1545,7 +1425,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9">
@@ -1566,7 +1446,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9">
@@ -1587,7 +1467,7 @@
         <v>8</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9">
@@ -1608,7 +1488,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9">
@@ -1629,7 +1509,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9">
@@ -1649,7 +1529,7 @@
     <row r="17" spans="1:10"/>
     <row r="18" spans="1:10">
       <c r="B18" s="10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -1658,7 +1538,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>

</xml_diff>

<commit_message>
fix select2 theme, fix status names, fix messages
</commit_message>
<xml_diff>
--- a/storage/app/reports/التقرير الأسبوعي-17.xlsx
+++ b/storage/app/reports/التقرير الأسبوعي-17.xlsx
@@ -33,13 +33,13 @@
     <t>صفحات الحفظ</t>
   </si>
   <si>
-    <t>18.18 %</t>
-  </si>
-  <si>
-    <t>نسبة الطلاب المجمدين</t>
-  </si>
-  <si>
-    <t>عدد الطلاب المجمدين</t>
+    <t>0.00 %</t>
+  </si>
+  <si>
+    <t>نسبة التجميد</t>
+  </si>
+  <si>
+    <t>عدد التجميد</t>
   </si>
   <si>
     <t>63.64 %</t>
@@ -60,24 +60,30 @@
     <t>نشط</t>
   </si>
   <si>
+    <t>نور الرحمن</t>
+  </si>
+  <si>
+    <t>ليس لديه مشرف</t>
+  </si>
+  <si>
+    <t>رامز شافع الخالدي</t>
+  </si>
+  <si>
+    <t>مجمد</t>
+  </si>
+  <si>
     <t>ليس ضمن حلقة</t>
   </si>
   <si>
-    <t>ليس لديه مشرف</t>
-  </si>
-  <si>
-    <t>رامز شافع الخالدي</t>
-  </si>
-  <si>
-    <t>مجمد</t>
-  </si>
-  <si>
     <t>مسؤول الطلاب للذكور</t>
   </si>
   <si>
     <t>مسؤول لجنة إعلامية</t>
   </si>
   <si>
+    <t>أحباب القرآن</t>
+  </si>
+  <si>
     <t>مشرف</t>
   </si>
   <si>
@@ -169,12 +175,6 @@
   </si>
   <si>
     <t>نور على نور</t>
-  </si>
-  <si>
-    <t>أحباب القرآن</t>
-  </si>
-  <si>
-    <t>نور الرحمن</t>
   </si>
   <si>
     <t>معدل النقاط</t>
@@ -232,7 +232,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +249,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFf2f2f2"/>
         <bgColor rgb="FFf2f2f2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFffe599"/>
+        <bgColor rgb="FFffe599"/>
       </patternFill>
     </fill>
     <fill>
@@ -309,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -326,7 +332,10 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="5" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="6" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="6" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="7" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -335,10 +344,10 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="7" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="8" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="8" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="9" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -650,7 +659,7 @@
   <sheetData>
     <row r="2" spans="1:12">
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -679,7 +688,7 @@
     <row r="4" spans="1:12"/>
     <row r="5" spans="1:12">
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -708,37 +717,37 @@
     <row r="7" spans="1:12"/>
     <row r="8" spans="1:12">
       <c r="B8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="K8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="L8" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -746,7 +755,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9" s="4">
         <v>26753970</v>
@@ -755,7 +764,7 @@
         <v>15</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>13</v>
@@ -781,7 +790,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D10" s="4">
         <v>22014233</v>
@@ -790,7 +799,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>13</v>
@@ -816,7 +825,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D11" s="4">
         <v>24264634</v>
@@ -825,7 +834,7 @@
         <v>15</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>13</v>
@@ -851,7 +860,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D12" s="4">
         <v>33480892</v>
@@ -860,7 +869,7 @@
         <v>15</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>13</v>
@@ -886,7 +895,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D13" s="4">
         <v>22012233</v>
@@ -895,7 +904,7 @@
         <v>15</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>13</v>
@@ -921,7 +930,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D14" s="4">
         <v>76107628</v>
@@ -930,7 +939,7 @@
         <v>15</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>13</v>
@@ -952,177 +961,177 @@
       </c>
     </row>
     <row r="15" spans="1:12">
-      <c r="B15" s="4">
+      <c r="B15" s="5">
         <v>7</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="5">
+        <v>22011233</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="4">
-        <v>22011233</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="G15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5">
+        <v>3</v>
+      </c>
+      <c r="J15" s="5">
+        <v>7</v>
+      </c>
+      <c r="K15" s="5">
+        <v>2</v>
+      </c>
+      <c r="L15" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="B16" s="6">
+        <v>8</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="6">
+        <v>22013233</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0</v>
+      </c>
+      <c r="J16" s="6">
+        <v>0</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="B17" s="6">
+        <v>9</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="6">
+        <v>22016233</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0</v>
+      </c>
+      <c r="I17" s="6">
+        <v>0</v>
+      </c>
+      <c r="J17" s="6">
+        <v>0</v>
+      </c>
+      <c r="K17" s="6">
+        <v>0</v>
+      </c>
+      <c r="L17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="B18" s="6">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="6">
+        <v>22017233</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0</v>
+      </c>
+      <c r="J18" s="6">
+        <v>0</v>
+      </c>
+      <c r="K18" s="6">
+        <v>0</v>
+      </c>
+      <c r="L18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="B19" s="6">
+        <v>11</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="6">
+        <v>28527252</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G19" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="4">
-        <v>1</v>
-      </c>
-      <c r="I15" s="4">
-        <v>3</v>
-      </c>
-      <c r="J15" s="4">
-        <v>7</v>
-      </c>
-      <c r="K15" s="4">
-        <v>2</v>
-      </c>
-      <c r="L15" s="4">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="B16" s="5">
-        <v>8</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="5">
-        <v>22013233</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0</v>
-      </c>
-      <c r="I16" s="5">
-        <v>0</v>
-      </c>
-      <c r="J16" s="5">
-        <v>0</v>
-      </c>
-      <c r="K16" s="5">
-        <v>0</v>
-      </c>
-      <c r="L16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="B17" s="5">
-        <v>9</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="5">
-        <v>22016233</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" s="5">
-        <v>0</v>
-      </c>
-      <c r="L17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
-      <c r="B18" s="5">
-        <v>10</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="5">
-        <v>22017233</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0</v>
-      </c>
-      <c r="I18" s="5">
-        <v>0</v>
-      </c>
-      <c r="J18" s="5">
-        <v>0</v>
-      </c>
-      <c r="K18" s="5">
-        <v>0</v>
-      </c>
-      <c r="L18" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="B19" s="5">
-        <v>11</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="5">
-        <v>28527252</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0</v>
-      </c>
-      <c r="I19" s="5">
-        <v>0</v>
-      </c>
-      <c r="J19" s="5">
-        <v>0</v>
-      </c>
-      <c r="K19" s="5">
-        <v>0</v>
-      </c>
-      <c r="L19" s="5">
+      <c r="H19" s="6">
+        <v>0</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0</v>
+      </c>
+      <c r="J19" s="6">
+        <v>0</v>
+      </c>
+      <c r="K19" s="6">
+        <v>0</v>
+      </c>
+      <c r="L19" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1157,79 +1166,79 @@
     </row>
     <row r="23" spans="1:12"/>
     <row r="24" spans="1:12">
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="7"/>
       <c r="D24" s="3">
         <v>11</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="7"/>
       <c r="G24" s="3">
         <v>7</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H24" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I24" s="6"/>
+      <c r="I24" s="7"/>
       <c r="J24" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:12">
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="6"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="3">
-        <v>2</v>
-      </c>
-      <c r="E25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F25" s="6"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H25" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I25" s="6"/>
+      <c r="I25" s="7"/>
       <c r="J25" s="3">
         <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:12">
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="7"/>
       <c r="D26" s="3">
         <v>19</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="7"/>
       <c r="G26" s="3">
         <v>1.73</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I26" s="6"/>
+      <c r="I26" s="7"/>
       <c r="J26" s="3">
         <v>1.73</v>
       </c>
     </row>
     <row r="27" spans="1:12">
-      <c r="B27" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="6"/>
+      <c r="B27" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="7"/>
       <c r="D27" s="3">
         <v>18.45</v>
       </c>
@@ -1270,279 +1279,279 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" spans="1:10">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10"/>
     <row r="5" spans="1:10">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8" t="s">
+      <c r="H5" s="9"/>
+      <c r="I5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="8"/>
+      <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="9">
+      <c r="B6" s="10">
         <v>1</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10">
+        <v>2</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10">
+        <v>9.5</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="B7" s="10">
+        <v>2</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8" s="10">
+        <v>3</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9">
-        <v>0</v>
-      </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="B7" s="9">
-        <v>2</v>
-      </c>
-      <c r="C7" s="9" t="s">
+      <c r="D8" s="10"/>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="J8" s="10"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="B9" s="10">
+        <v>4</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9">
-        <v>0</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="B8" s="9">
-        <v>3</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="D9" s="10"/>
+      <c r="E9" s="10">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" s="10">
+        <v>5</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9">
-        <v>0</v>
-      </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="B9" s="9">
-        <v>4</v>
-      </c>
-      <c r="C9" s="9" t="s">
+      <c r="D10" s="10"/>
+      <c r="E10" s="10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" s="10">
+        <v>6</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9">
-        <v>0</v>
-      </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="B10" s="9">
-        <v>5</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="D11" s="10"/>
+      <c r="E11" s="10">
+        <v>0</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="J11" s="10"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" s="10">
+        <v>7</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9">
-        <v>0</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="B11" s="9">
-        <v>6</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="D12" s="10"/>
+      <c r="E12" s="10">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="J12" s="10"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="10">
+        <v>8</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9">
-        <v>0</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="B12" s="9">
-        <v>7</v>
-      </c>
-      <c r="C12" s="9" t="s">
+      <c r="D13" s="10"/>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="J13" s="10"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" s="10">
+        <v>9</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9">
-        <v>0</v>
-      </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="B13" s="9">
-        <v>8</v>
-      </c>
-      <c r="C13" s="9" t="s">
+      <c r="D14" s="10"/>
+      <c r="E14" s="10">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" s="10">
+        <v>10</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9">
-        <v>0</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="B14" s="9">
-        <v>9</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9">
-        <v>0</v>
-      </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="B15" s="9">
-        <v>10</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9">
-        <v>0</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="J15" s="9"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10">
+        <v>0</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10">
+        <v>0.0</v>
+      </c>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10"/>
     <row r="17" spans="1:10"/>
     <row r="18" spans="1:10">
-      <c r="B18" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="8">
-        <v>0</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="8">
+      <c r="B18" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="9">
+        <v>0</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="9">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>